<commit_message>
adding fourth corner analysis
</commit_message>
<xml_diff>
--- a/traits.xlsx
+++ b/traits.xlsx
@@ -5,16 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mendelu-my.sharepoint.com/personal/xstoces_mendelu_cz1/Documents/SSD_21.12.2024/Caha_sady/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominik\Apple-orchards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_AD4D80C4656A4B7AC02E7484B35F43565BDEDD8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF6B09F3-328C-4306-877E-AB6A6FB9EFB4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EB51FC-65BA-410D-88B4-6D939BE3D3FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2625" yWindow="345" windowWidth="20040" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26685" yWindow="150" windowWidth="24915" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">List1!$A$1:$G$478</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1688,8 +1691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G478"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A323" workbookViewId="0">
+      <selection activeCell="D326" sqref="D326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9684,6 +9687,7 @@
       <c r="F478" s="4"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G478" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>